<commit_message>
Modification de la conceptMap 09bc5b4cb8eba29a1df71f31a626cb87650d9a34
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/documentReferenceToMHD.xlsx
+++ b/add-info-dmp/ig/documentReferenceToMHD.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-30T14:55:26+00:00</t>
+    <t>2025-04-30T15:08:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -108,13 +108,67 @@
     <t>https://interop.esante.gouv.fr/ig/fhir/pdsm/StructureDefinition/pdsm-comprehensive-document-reference</t>
   </si>
   <si>
+    <t>DocumentEntry.entryUUID</t>
+  </si>
+  <si>
+    <t>equivalent</t>
+  </si>
+  <si>
+    <t>DocumentReference.id</t>
+  </si>
+  <si>
+    <t>DocumentEntry.logicalId</t>
+  </si>
+  <si>
+    <t>DocumentReference.identifier</t>
+  </si>
+  <si>
+    <t>DocumentEntry.hash</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.hash</t>
+  </si>
+  <si>
+    <t>DocumentEntry.size</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.size</t>
+  </si>
+  <si>
+    <t>DocumentEntry.languageCode</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.language</t>
+  </si>
+  <si>
+    <t>DocumentEntry.legalAuthenticator</t>
+  </si>
+  <si>
+    <t>DocumentReference.authenticator</t>
+  </si>
+  <si>
+    <t>DocumentEntry.serviceStartTime</t>
+  </si>
+  <si>
+    <t>DocumentReference.context.period.start</t>
+  </si>
+  <si>
+    <t>DocumentEntry.serviceEndTime</t>
+  </si>
+  <si>
+    <t>DocumentReference.context.period.end</t>
+  </si>
+  <si>
+    <t>DocumentEntry.sourcePatientID</t>
+  </si>
+  <si>
+    <t>DocumentReference.subject.fr-core-patient</t>
+  </si>
+  <si>
+    <t>DocumentEntry.sourcePatientInfo</t>
+  </si>
+  <si>
     <t>DocumentEntry.URI</t>
-  </si>
-  <si>
-    <t>equivalent</t>
-  </si>
-  <si>
-    <t>DocumentReference.subject.fr-core-patient</t>
   </si>
   <si>
     <t>DocumentEntry.title</t>
@@ -416,7 +470,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -477,100 +531,118 @@
       <c r="C4" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" t="s" s="2">
+        <v>35</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" t="s" s="2">
+        <v>37</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" t="s" s="2">
+        <v>39</v>
+      </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" t="s" s="2">
+        <v>47</v>
+      </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" t="s" s="2">
+        <v>49</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" t="s" s="2">
+        <v>49</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -581,7 +653,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -592,7 +664,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -603,7 +675,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -614,7 +686,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -625,7 +697,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -636,7 +708,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -644,6 +716,116 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>